<commit_message>
# update cummins program commit.
</commit_message>
<xml_diff>
--- a/jsreg.xlsx
+++ b/jsreg.xlsx
@@ -115,6 +115,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -140,7 +141,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -151,6 +152,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,7 +457,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -535,6 +539,9 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="4">
+        <v>41194</v>
+      </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>

</xml_diff>